<commit_message>
addded combined report or anova + new partcipatns
Signed-off-by: aditya sahu <ad2004sahu@gmail.com>
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Acads\mtp\Data_Analsysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987E231-1998-458C-AD5A-EA2A32F40C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14C9EDE-CA61-43F6-A451-A48F3DE9D111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C98BBE88-DDF9-4139-BA41-8750DB938C4A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -510,13 +511,34 @@
   </si>
   <si>
     <t>B24216</t>
+  </si>
+  <si>
+    <t>Shivam Jaiswal</t>
+  </si>
+  <si>
+    <t>Sanskriti Sahu</t>
+  </si>
+  <si>
+    <t>Denny H Konyak</t>
+  </si>
+  <si>
+    <t>Rishabh Raj</t>
+  </si>
+  <si>
+    <t>CS-303</t>
+  </si>
+  <si>
+    <t>Compensation</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -622,8 +644,13 @@
       <color rgb="FF444746"/>
       <name val="Google Sans"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,12 +703,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -740,16 +761,16 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="7" xr:uid="{2F91BCE5-DC96-426B-BD35-5D2120CA3ACB}"/>
@@ -1105,15 +1126,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575A4C8F-9D59-4D9E-85B0-2E0FF6292F0A}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77:B80"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="5" width="12.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1129,1135 +1151,1376 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="E7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="5">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="5">
         <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21">
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22">
+      <c r="E22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>64</v>
+        <v>39</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
+      <c r="E35" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
+      <c r="E38" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>73</v>
+        <v>44</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>75</v>
+        <v>45</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
+      <c r="E40" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>77</v>
+        <v>46</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>79</v>
+        <v>47</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>85</v>
+        <v>50</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>87</v>
+        <v>51</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>104</v>
+        <v>52</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
+      <c r="E47" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>99</v>
+        <v>54</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>103</v>
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="D50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>106</v>
+        <v>56</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>57</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>110</v>
+        <v>58</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="D53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>112</v>
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>114</v>
+        <v>60</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="D55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>116</v>
+        <v>61</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="D56">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>118</v>
+        <v>62</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="D57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>120</v>
+        <v>63</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D59">
+      <c r="E59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>65</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D60">
+      <c r="E60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>66</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D61">
+      <c r="E61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>67</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D62">
+      <c r="E62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.25">
+      <c r="A63">
+        <v>68</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D63">
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>70</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D64" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D64">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>134</v>
+        <v>71</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>155</v>
+        <v>72</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>136</v>
+        <v>73</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="D67">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>138</v>
+        <v>74</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="14.25">
+      <c r="E68" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>140</v>
+        <v>75</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="D69">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70">
+        <v>76</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C70" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>67</v>
+      </c>
+      <c r="F71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>89</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>35</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>41</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
         <v>69</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C77" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D70">
+      <c r="D77">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D71" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D72">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="C77" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="B78" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D78">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="B79" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>156</v>
       </c>
       <c r="D79">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="C80" t="s">
         <v>158</v>
       </c>
       <c r="D80">
         <v>4</v>
       </c>
+      <c r="E80" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F80">
+    <sortCondition ref="E1:E80"/>
+  </sortState>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>